<commit_message>
Competition task - Extent Report using XML pending
</commit_message>
<xml_diff>
--- a/Competition/Competition/ExcelData/ExcelData.xlsx
+++ b/Competition/Competition/ExcelData/ExcelData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Industry Connect\Internship\Tasks\MarsQA-2\Competition\Competition\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94FB226F-D0D3-4987-8AEB-F7D8B14FE5F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEF6D17D-3964-4F64-880F-93E10E39F48F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{82EEA056-9B79-4A10-8889-AA867495E780}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{82EEA056-9B79-4A10-8889-AA867495E780}"/>
   </bookViews>
   <sheets>
     <sheet name="LogIn" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="72">
   <si>
     <t>charlie.penaredondo@gmail.com</t>
   </si>
@@ -97,9 +97,6 @@
     <t>Programming &amp; Tech</t>
   </si>
   <si>
-    <t>Tester</t>
-  </si>
-  <si>
     <t>Hourly basis service</t>
   </si>
   <si>
@@ -127,9 +124,6 @@
     <t>Skill Trade</t>
   </si>
   <si>
-    <t>Exchange TAG</t>
-  </si>
-  <si>
     <t>Service Type</t>
   </si>
   <si>
@@ -139,12 +133,6 @@
     <t>8:30pm</t>
   </si>
   <si>
-    <t>Edit Test Automation</t>
-  </si>
-  <si>
-    <t>Edit Quality Assurance and Test Automation Services</t>
-  </si>
-  <si>
     <t>Wed</t>
   </si>
   <si>
@@ -154,27 +142,12 @@
     <t>10:30pm</t>
   </si>
   <si>
-    <t>Edit TAG TAG</t>
-  </si>
-  <si>
     <t>Mon</t>
   </si>
   <si>
     <t>Skill-exchange</t>
   </si>
   <si>
-    <t>TestRow</t>
-  </si>
-  <si>
-    <t>Test from Row 2</t>
-  </si>
-  <si>
-    <t>Testfromrow3</t>
-  </si>
-  <si>
-    <t>Row3</t>
-  </si>
-  <si>
     <t>Digital Marketing</t>
   </si>
   <si>
@@ -182,6 +155,105 @@
   </si>
   <si>
     <t>One-off service</t>
+  </si>
+  <si>
+    <t>Work Sample</t>
+  </si>
+  <si>
+    <t>wink.png</t>
+  </si>
+  <si>
+    <t>lol.png</t>
+  </si>
+  <si>
+    <t>smile.png</t>
+  </si>
+  <si>
+    <t>cry.png</t>
+  </si>
+  <si>
+    <t>Content Marketing Expert</t>
+  </si>
+  <si>
+    <t>On-site</t>
+  </si>
+  <si>
+    <t>DevOps</t>
+  </si>
+  <si>
+    <t>Photoshop</t>
+  </si>
+  <si>
+    <t>Web Design</t>
+  </si>
+  <si>
+    <t>Software Testing</t>
+  </si>
+  <si>
+    <t>Video &amp; Animation</t>
+  </si>
+  <si>
+    <t>Digital Creator</t>
+  </si>
+  <si>
+    <t>Editing &amp; Post Production</t>
+  </si>
+  <si>
+    <t>Videographer</t>
+  </si>
+  <si>
+    <t>Video and Animation Expert</t>
+  </si>
+  <si>
+    <t>Lightroom</t>
+  </si>
+  <si>
+    <t>8:30am</t>
+  </si>
+  <si>
+    <t>5:30pm</t>
+  </si>
+  <si>
+    <t>Music</t>
+  </si>
+  <si>
+    <t>Negative Test</t>
+  </si>
+  <si>
+    <t>Edited Test Automation</t>
+  </si>
+  <si>
+    <t>Edited  Digital Creator</t>
+  </si>
+  <si>
+    <t>Edited  Videographer</t>
+  </si>
+  <si>
+    <t>Edited Negative Test</t>
+  </si>
+  <si>
+    <t>Edited Content Marketing Expert</t>
+  </si>
+  <si>
+    <t>Edited Quality Assurance and Test Automation Services</t>
+  </si>
+  <si>
+    <t>Edited Video and Animation Expert</t>
+  </si>
+  <si>
+    <t>Tue</t>
+  </si>
+  <si>
+    <t>Thur</t>
+  </si>
+  <si>
+    <t>Edit DevOps</t>
+  </si>
+  <si>
+    <t>Edit Photoshop</t>
+  </si>
+  <si>
+    <t>Edit Music</t>
   </si>
 </sst>
 </file>
@@ -601,10 +673,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18D89DED-8D1F-4B5A-8409-5FB4BAD54529}">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,7 +685,7 @@
     <col min="2" max="2" width="44.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1"/>
     <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
@@ -626,7 +698,7 @@
     <col min="16" max="16" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -643,7 +715,7 @@
         <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G1" t="s">
         <v>11</v>
@@ -655,19 +727,19 @@
         <v>13</v>
       </c>
       <c r="J1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="M1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O1" t="s">
         <v>15</v>
@@ -675,8 +747,11 @@
       <c r="P1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -687,16 +762,16 @@
         <v>18</v>
       </c>
       <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
         <v>24</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" t="s">
-        <v>25</v>
       </c>
       <c r="H2" s="3">
         <v>45067</v>
@@ -705,48 +780,51 @@
         <v>45127</v>
       </c>
       <c r="J2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="N2" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="O2">
         <v>2</v>
       </c>
       <c r="P2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
         <v>44</v>
       </c>
       <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" t="s">
         <v>45</v>
-      </c>
-      <c r="D3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G3" t="s">
-        <v>25</v>
       </c>
       <c r="H3" s="3">
         <v>45128</v>
@@ -755,25 +833,98 @@
         <v>45189</v>
       </c>
       <c r="J3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="N3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="O3">
         <v>3</v>
       </c>
       <c r="P3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="3">
+        <v>45107</v>
+      </c>
+      <c r="I4" s="3">
+        <v>45214</v>
+      </c>
+      <c r="J4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N4" t="s">
+        <v>58</v>
+      </c>
+      <c r="O4">
+        <v>4</v>
+      </c>
+      <c r="P4" t="s">
         <v>14</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="3">
+        <v>45214</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -784,10 +935,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E942612B-DA7F-4F32-91A3-658E3314CC20}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -809,7 +960,7 @@
     <col min="16" max="16" width="6.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -826,7 +977,7 @@
         <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G1" t="s">
         <v>11</v>
@@ -838,19 +989,19 @@
         <v>13</v>
       </c>
       <c r="J1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="M1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O1" t="s">
         <v>15</v>
@@ -858,56 +1009,188 @@
       <c r="P1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
       </c>
       <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" s="3">
+        <v>45076</v>
+      </c>
+      <c r="I2" s="3">
+        <v>45108</v>
+      </c>
+      <c r="J2" t="s">
+        <v>67</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N2" t="s">
+        <v>69</v>
+      </c>
+      <c r="O2">
+        <v>5</v>
+      </c>
+      <c r="P2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
         <v>24</v>
       </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="3">
-        <v>45067</v>
-      </c>
-      <c r="I2" s="3">
-        <v>45127</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="H3" s="3">
+        <v>45123</v>
+      </c>
+      <c r="I3" s="3">
+        <v>45191</v>
+      </c>
+      <c r="J3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="N3" t="s">
+        <v>70</v>
+      </c>
+      <c r="O3">
+        <v>3</v>
+      </c>
+      <c r="P3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="3">
+        <v>45079</v>
+      </c>
+      <c r="I4" s="3">
+        <v>45208</v>
+      </c>
+      <c r="J4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="M4" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="N4" t="s">
+        <v>71</v>
+      </c>
+      <c r="O4">
+        <v>2</v>
+      </c>
+      <c r="P4" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" t="s">
         <v>38</v>
       </c>
-      <c r="O2">
-        <v>25</v>
-      </c>
-      <c r="P2" t="s">
-        <v>14</v>
-      </c>
+      <c r="G5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="3">
+        <v>45214</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H6" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
MarsQA - Competition Task
</commit_message>
<xml_diff>
--- a/Competition/Competition/ExcelData/ExcelData.xlsx
+++ b/Competition/Competition/ExcelData/ExcelData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Industry Connect\Internship\Tasks\MarsQA-2\Competition\Competition\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEF6D17D-3964-4F64-880F-93E10E39F48F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71718554-7CA3-4372-9507-CE9D52352802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{82EEA056-9B79-4A10-8889-AA867495E780}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{82EEA056-9B79-4A10-8889-AA867495E780}"/>
   </bookViews>
   <sheets>
     <sheet name="LogIn" sheetId="2" r:id="rId1"/>
@@ -76,9 +76,6 @@
     <t>Location Type</t>
   </si>
   <si>
-    <t>Start date</t>
-  </si>
-  <si>
     <t>End Date</t>
   </si>
   <si>
@@ -100,15 +97,6 @@
     <t>Hourly basis service</t>
   </si>
   <si>
-    <t>Start day</t>
-  </si>
-  <si>
-    <t>Start time</t>
-  </si>
-  <si>
-    <t>End time</t>
-  </si>
-  <si>
     <t>QA</t>
   </si>
   <si>
@@ -254,6 +242,18 @@
   </si>
   <si>
     <t>Edit Music</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>Start Day</t>
+  </si>
+  <si>
+    <t>Start Time</t>
+  </si>
+  <si>
+    <t>End Time</t>
   </si>
 </sst>
 </file>
@@ -675,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18D89DED-8D1F-4B5A-8409-5FB4BAD54529}">
   <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:Q6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,63 +715,63 @@
         <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G1" t="s">
         <v>11</v>
       </c>
       <c r="H1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="M1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="M1" t="s">
-        <v>27</v>
-      </c>
-      <c r="N1" t="s">
-        <v>25</v>
-      </c>
-      <c r="O1" t="s">
-        <v>15</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
       <c r="Q1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>17</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" t="s">
         <v>18</v>
       </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F2" t="s">
-        <v>19</v>
-      </c>
       <c r="G2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H2" s="3">
         <v>45067</v>
@@ -780,51 +780,51 @@
         <v>45127</v>
       </c>
       <c r="J2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="N2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="O2">
         <v>2</v>
       </c>
       <c r="P2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s">
         <v>44</v>
       </c>
-      <c r="C3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" t="s">
-        <v>48</v>
-      </c>
       <c r="F3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="H3" s="3">
         <v>45128</v>
@@ -833,51 +833,51 @@
         <v>45189</v>
       </c>
       <c r="J3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="O3">
         <v>3</v>
       </c>
       <c r="P3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="Q3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H4" s="3">
         <v>45107</v>
@@ -886,45 +886,45 @@
         <v>45214</v>
       </c>
       <c r="J4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="M4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>35</v>
-      </c>
       <c r="N4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="O4">
         <v>4</v>
       </c>
       <c r="P4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="I5" s="3">
         <v>45214</v>
       </c>
       <c r="Q5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -937,8 +937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E942612B-DA7F-4F32-91A3-658E3314CC20}">
   <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -977,63 +977,63 @@
         <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G1" t="s">
         <v>11</v>
       </c>
       <c r="H1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="M1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="M1" t="s">
-        <v>27</v>
-      </c>
-      <c r="N1" t="s">
-        <v>25</v>
-      </c>
-      <c r="O1" t="s">
-        <v>15</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
       <c r="Q1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="H2" s="3">
         <v>45076</v>
@@ -1042,51 +1042,51 @@
         <v>45108</v>
       </c>
       <c r="J2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="N2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="O2">
         <v>5</v>
       </c>
       <c r="P2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="Q2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H3" s="3">
         <v>45123</v>
@@ -1095,51 +1095,51 @@
         <v>45191</v>
       </c>
       <c r="J3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="O3">
         <v>3</v>
       </c>
       <c r="P3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" t="s">
         <v>62</v>
       </c>
-      <c r="B4" t="s">
-        <v>66</v>
-      </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H4" s="3">
         <v>45079</v>
@@ -1148,45 +1148,45 @@
         <v>45208</v>
       </c>
       <c r="J4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="M4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>35</v>
-      </c>
       <c r="N4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="O4">
         <v>2</v>
       </c>
       <c r="P4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="I5" s="3">
         <v>45214</v>
       </c>
       <c r="Q5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Revisions, Negative Tests, Signup
</commit_message>
<xml_diff>
--- a/Competition/Competition/ExcelData/ExcelData.xlsx
+++ b/Competition/Competition/ExcelData/ExcelData.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Industry Connect\Internship\Tasks\MarsQA-2\Competition\Competition\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71718554-7CA3-4372-9507-CE9D52352802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C749A5-1470-4E5E-915B-FCE73583CE1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{82EEA056-9B79-4A10-8889-AA867495E780}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{82EEA056-9B79-4A10-8889-AA867495E780}"/>
   </bookViews>
   <sheets>
     <sheet name="LogIn" sheetId="2" r:id="rId1"/>
     <sheet name="ShareSkill" sheetId="3" r:id="rId2"/>
-    <sheet name="ManageListings" sheetId="4" r:id="rId3"/>
+    <sheet name="Signup" sheetId="5" r:id="rId3"/>
+    <sheet name="ManageListings" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="83">
   <si>
     <t>charlie.penaredondo@gmail.com</t>
   </si>
@@ -49,9 +50,6 @@
     <t>UserEmail</t>
   </si>
   <si>
-    <t>password</t>
-  </si>
-  <si>
     <t>http://localhost:5000/</t>
   </si>
   <si>
@@ -181,18 +179,9 @@
     <t>Video &amp; Animation</t>
   </si>
   <si>
-    <t>Digital Creator</t>
-  </si>
-  <si>
     <t>Editing &amp; Post Production</t>
   </si>
   <si>
-    <t>Videographer</t>
-  </si>
-  <si>
-    <t>Video and Animation Expert</t>
-  </si>
-  <si>
     <t>Lightroom</t>
   </si>
   <si>
@@ -254,6 +243,51 @@
   </si>
   <si>
     <t>End Time</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Charlie</t>
+  </si>
+  <si>
+    <t>Penaredondo</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>password123123</t>
+  </si>
+  <si>
+    <t>Production</t>
+  </si>
+  <si>
+    <t>100 characters blah blah 100 characters blah blah100 characters blah blah100 characters blah blah100 characters blah blah100 characters blah blah100 characters blah blah</t>
+  </si>
+  <si>
+    <t>TestUpload.pptx</t>
+  </si>
+  <si>
+    <t>No Desc Test</t>
+  </si>
+  <si>
+    <t>No Category Test</t>
+  </si>
+  <si>
+    <t>No SubCategory Test</t>
+  </si>
+  <si>
+    <t>No Tags Test</t>
+  </si>
+  <si>
+    <t>Speci@l Character test. I am a Videographer and I'm writing a titile over 100 with special char@cters. I r3@lly H0pe th@t this test will p@$$. B;lah blah blah blah</t>
+  </si>
+  <si>
+    <t>Wrong File Format Test</t>
   </si>
 </sst>
 </file>
@@ -629,10 +663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37BED2C8-AAC0-4E2C-BC24-D084745FF497}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,29 +677,41 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{FDD801EA-2ECE-4C75-8BA3-9694A61B8925}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{12C41B65-AAA0-4586-A9F6-085A3264820C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -673,10 +719,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18D89DED-8D1F-4B5A-8409-5FB4BAD54529}">
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection sqref="A1:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,7 +731,7 @@
     <col min="2" max="2" width="44.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
@@ -699,79 +745,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
-        <v>68</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="M1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" t="s">
-        <v>69</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="M1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N1" t="s">
-        <v>21</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>19</v>
-      </c>
-      <c r="E2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" t="s">
-        <v>20</v>
       </c>
       <c r="H2" s="3">
         <v>45067</v>
@@ -780,51 +826,49 @@
         <v>45127</v>
       </c>
       <c r="J2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>31</v>
-      </c>
       <c r="N2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O2">
         <v>2</v>
       </c>
       <c r="P2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Q2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" t="s">
         <v>40</v>
-      </c>
-      <c r="C3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G3" t="s">
-        <v>41</v>
       </c>
       <c r="H3" s="3">
         <v>45128</v>
@@ -833,51 +877,49 @@
         <v>45189</v>
       </c>
       <c r="J3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="L3" s="6" t="s">
-        <v>29</v>
-      </c>
       <c r="M3" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O3">
         <v>3</v>
       </c>
       <c r="P3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Q3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="A4" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" t="s">
-        <v>51</v>
+      <c r="E4" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H4" s="3">
         <v>45107</v>
@@ -886,45 +928,340 @@
         <v>45214</v>
       </c>
       <c r="J4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="O4">
         <v>4</v>
       </c>
       <c r="P4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Q4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>55</v>
+      <c r="A5" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>74</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="H5" s="3">
+        <v>45107</v>
       </c>
       <c r="I5" s="3">
         <v>45214</v>
       </c>
+      <c r="J5" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N5" t="s">
+        <v>50</v>
+      </c>
+      <c r="O5">
+        <v>4</v>
+      </c>
+      <c r="P5" t="s">
+        <v>12</v>
+      </c>
       <c r="Q5" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="3">
+        <v>45107</v>
+      </c>
+      <c r="I6" s="3">
+        <v>45214</v>
+      </c>
+      <c r="J6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N6" t="s">
+        <v>50</v>
+      </c>
+      <c r="O6">
+        <v>4</v>
+      </c>
+      <c r="P6" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="3">
+        <v>45107</v>
+      </c>
+      <c r="I7" s="3">
+        <v>45214</v>
+      </c>
+      <c r="J7" t="s">
+        <v>26</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N7" t="s">
+        <v>50</v>
+      </c>
+      <c r="O7">
+        <v>4</v>
+      </c>
+      <c r="P7" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="F8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="3">
+        <v>45107</v>
+      </c>
+      <c r="I8" s="3">
+        <v>45214</v>
+      </c>
+      <c r="J8" t="s">
+        <v>26</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N8" t="s">
+        <v>50</v>
+      </c>
+      <c r="O8">
+        <v>4</v>
+      </c>
+      <c r="P8" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="F9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" s="3">
+        <v>45107</v>
+      </c>
+      <c r="I9" s="3">
+        <v>45214</v>
+      </c>
+      <c r="J9" t="s">
+        <v>26</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N9" t="s">
+        <v>50</v>
+      </c>
+      <c r="O9">
+        <v>4</v>
+      </c>
+      <c r="P9" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="F10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="3">
+        <v>45107</v>
+      </c>
+      <c r="I10" s="3">
+        <v>45214</v>
+      </c>
+      <c r="J10" t="s">
+        <v>26</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N10" t="s">
+        <v>50</v>
+      </c>
+      <c r="O10">
+        <v>4</v>
+      </c>
+      <c r="P10" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -934,6 +1271,58 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF996530-E5D2-4E22-A138-58BA738E3C19}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="3" max="3" width="30" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{E9E2A182-8A83-419A-98B6-0CFB30569639}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E942612B-DA7F-4F32-91A3-658E3314CC20}">
   <dimension ref="A1:Q6"/>
   <sheetViews>
@@ -962,78 +1351,78 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
-        <v>68</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="M1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" t="s">
-        <v>69</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="M1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N1" t="s">
-        <v>21</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>13</v>
-      </c>
       <c r="Q1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H2" s="3">
         <v>45076</v>
@@ -1042,51 +1431,51 @@
         <v>45108</v>
       </c>
       <c r="J2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="O2">
         <v>5</v>
       </c>
       <c r="P2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Q2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
         <v>32</v>
       </c>
-      <c r="D3" t="s">
-        <v>33</v>
-      </c>
       <c r="E3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H3" s="3">
         <v>45123</v>
@@ -1095,51 +1484,51 @@
         <v>45191</v>
       </c>
       <c r="J3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="O3">
         <v>3</v>
       </c>
       <c r="P3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Q3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" t="s">
         <v>58</v>
       </c>
-      <c r="B4" t="s">
-        <v>62</v>
-      </c>
       <c r="C4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" t="s">
         <v>46</v>
       </c>
-      <c r="D4" t="s">
-        <v>48</v>
-      </c>
       <c r="E4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H4" s="3">
         <v>45079</v>
@@ -1148,45 +1537,45 @@
         <v>45208</v>
       </c>
       <c r="J4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="O4">
         <v>2</v>
       </c>
       <c r="P4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Q4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I5" s="3">
         <v>45214</v>
       </c>
       <c r="Q5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>